<commit_message>
Added table_1b_by_subject.csv and fixed metadata for table_1b_by_gender.csv
</commit_message>
<xml_diff>
--- a/data/processed/01_stage_1/SFR01_2014_NT.xlsx
+++ b/data/processed/01_stage_1/SFR01_2014_NT.xlsx
@@ -9,6 +9,7 @@
   <sheets>
     <sheet name="table_1a.csv" sheetId="1" r:id="rId1"/>
     <sheet name="table_1b_by_gender.csv" sheetId="2" r:id="rId2"/>
+    <sheet name="table_1b_by_subject.csv" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="49">
   <si>
     <t>15 year olds</t>
   </si>
@@ -143,13 +144,52 @@
   </si>
   <si>
     <t>perc_achieved_statefunded_2012</t>
+  </si>
+  <si>
+    <t>English</t>
+  </si>
+  <si>
+    <t>Mathematics</t>
+  </si>
+  <si>
+    <t>subject</t>
+  </si>
+  <si>
+    <t>Sciences - Not triple science</t>
+  </si>
+  <si>
+    <r>
+      <t>Sciences - triple science</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <vertAlign val="superscript"/>
+        <sz val="8"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>5</t>
+    </r>
+  </si>
+  <si>
+    <t>History or Geography</t>
+  </si>
+  <si>
+    <t>Languages</t>
+  </si>
+  <si>
+    <t>gender</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.0"/>
+  </numFmts>
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -159,6 +199,11 @@
     </font>
     <font>
       <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -194,6 +239,19 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="8"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <i/>
+      <vertAlign val="superscript"/>
+      <sz val="8"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -251,162 +309,234 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="90">
+  <cellStyleXfs count="130">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" indent="2"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="2"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="2"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="2"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="3"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="90">
+  <cellStyles count="130">
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
@@ -451,6 +581,26 @@
     <cellStyle name="Followed Hyperlink" xfId="85" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="87" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="89" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="91" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="93" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="95" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="97" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="99" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="101" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="103" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="105" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="107" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="109" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="111" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="113" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="115" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="117" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="119" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="121" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="123" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="125" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="127" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="129" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="6" builtinId="8" hidden="1"/>
@@ -495,6 +645,26 @@
     <cellStyle name="Hyperlink" xfId="84" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="86" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="88" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="90" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="92" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="94" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="96" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="98" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="100" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="102" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="104" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="106" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="108" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="110" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="112" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="114" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="116" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="118" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="120" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="122" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="124" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="126" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="128" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2 2" xfId="1"/>
   </cellStyles>
@@ -835,7 +1005,7 @@
   <cols>
     <col min="1" max="1" width="30.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="21.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="8" width="10.83203125" style="15"/>
+    <col min="3" max="8" width="10.83203125" style="17"/>
     <col min="9" max="9" width="45" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -846,25 +1016,25 @@
       <c r="B1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="C1" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="D1" s="16" t="s">
+      <c r="D1" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="E1" s="16" t="s">
+      <c r="E1" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="F1" s="16" t="s">
+      <c r="F1" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="G1" s="16" t="s">
+      <c r="G1" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="H1" s="16" t="s">
+      <c r="H1" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="I1" s="9" t="s">
+      <c r="I1" s="11" t="s">
         <v>3</v>
       </c>
     </row>
@@ -875,22 +1045,22 @@
       <c r="B2" s="3">
         <v>1995</v>
       </c>
-      <c r="C2" s="11">
+      <c r="C2" s="13">
         <v>594035</v>
       </c>
-      <c r="D2" s="12">
+      <c r="D2" s="14">
         <v>44.5</v>
       </c>
-      <c r="E2" s="12">
+      <c r="E2" s="14">
         <v>35.200000000000003</v>
       </c>
-      <c r="F2" s="12">
+      <c r="F2" s="14">
         <v>86.1</v>
       </c>
-      <c r="G2" s="12">
+      <c r="G2" s="14">
         <v>83.4</v>
       </c>
-      <c r="H2" s="12">
+      <c r="H2" s="14">
         <v>92.2</v>
       </c>
       <c r="I2" t="s">
@@ -904,22 +1074,22 @@
       <c r="B3" s="3">
         <v>1996</v>
       </c>
-      <c r="C3" s="11">
+      <c r="C3" s="13">
         <v>586766</v>
       </c>
-      <c r="D3" s="12">
+      <c r="D3" s="14">
         <v>45.1</v>
       </c>
-      <c r="E3" s="11">
+      <c r="E3" s="13">
         <v>35.6</v>
       </c>
-      <c r="F3" s="12">
+      <c r="F3" s="14">
         <v>86.4</v>
       </c>
-      <c r="G3" s="12">
+      <c r="G3" s="14">
         <v>83.9</v>
       </c>
-      <c r="H3" s="12">
+      <c r="H3" s="14">
         <v>92.3</v>
       </c>
     </row>
@@ -930,22 +1100,22 @@
       <c r="B4" s="3">
         <v>1997</v>
       </c>
-      <c r="C4" s="11">
+      <c r="C4" s="13">
         <v>575210</v>
       </c>
-      <c r="D4" s="12">
+      <c r="D4" s="14">
         <v>46.3</v>
       </c>
-      <c r="E4" s="11">
+      <c r="E4" s="13">
         <v>37</v>
       </c>
-      <c r="F4" s="12">
+      <c r="F4" s="14">
         <v>87.5</v>
       </c>
-      <c r="G4" s="12">
+      <c r="G4" s="14">
         <v>83.8</v>
       </c>
-      <c r="H4" s="12">
+      <c r="H4" s="14">
         <v>93.4</v>
       </c>
     </row>
@@ -956,22 +1126,22 @@
       <c r="B5" s="3">
         <v>1998</v>
       </c>
-      <c r="C5" s="11">
+      <c r="C5" s="13">
         <v>580972</v>
       </c>
-      <c r="D5" s="11">
+      <c r="D5" s="13">
         <v>47.9</v>
       </c>
-      <c r="E5" s="11">
+      <c r="E5" s="13">
         <v>38.6</v>
       </c>
-      <c r="F5" s="11">
+      <c r="F5" s="13">
         <v>88.5</v>
       </c>
-      <c r="G5" s="11">
+      <c r="G5" s="13">
         <v>85.8</v>
       </c>
-      <c r="H5" s="11">
+      <c r="H5" s="13">
         <v>94</v>
       </c>
     </row>
@@ -979,25 +1149,25 @@
       <c r="A6" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B6" s="4">
+      <c r="B6" s="5">
         <v>1999</v>
       </c>
-      <c r="C6" s="12">
+      <c r="C6" s="14">
         <v>580393</v>
       </c>
-      <c r="D6" s="12">
+      <c r="D6" s="14">
         <v>49.2</v>
       </c>
-      <c r="E6" s="11">
+      <c r="E6" s="13">
         <v>40</v>
       </c>
-      <c r="F6" s="12">
+      <c r="F6" s="14">
         <v>88.9</v>
       </c>
-      <c r="G6" s="12">
+      <c r="G6" s="14">
         <v>86.8</v>
       </c>
-      <c r="H6" s="12">
+      <c r="H6" s="14">
         <v>94.4</v>
       </c>
     </row>
@@ -1005,25 +1175,25 @@
       <c r="A7" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B7" s="4">
+      <c r="B7" s="5">
         <v>2000</v>
       </c>
-      <c r="C7" s="12">
+      <c r="C7" s="14">
         <v>603318</v>
       </c>
-      <c r="D7" s="12">
+      <c r="D7" s="14">
         <v>50</v>
       </c>
-      <c r="E7" s="11">
+      <c r="E7" s="13">
         <v>40.700000000000003</v>
       </c>
-      <c r="F7" s="12">
+      <c r="F7" s="14">
         <v>88.9</v>
       </c>
-      <c r="G7" s="12">
+      <c r="G7" s="14">
         <v>86.9</v>
       </c>
-      <c r="H7" s="12">
+      <c r="H7" s="14">
         <v>94.5</v>
       </c>
     </row>
@@ -1031,25 +1201,25 @@
       <c r="A8" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B8" s="4">
+      <c r="B8" s="5">
         <v>2001</v>
       </c>
-      <c r="C8" s="12">
+      <c r="C8" s="14">
         <v>606554</v>
       </c>
-      <c r="D8" s="12">
+      <c r="D8" s="14">
         <v>51.6</v>
       </c>
-      <c r="E8" s="11">
+      <c r="E8" s="13">
         <v>42.1</v>
       </c>
-      <c r="F8" s="12">
+      <c r="F8" s="14">
         <v>88.9</v>
       </c>
-      <c r="G8" s="12">
+      <c r="G8" s="14">
         <v>87.1</v>
       </c>
-      <c r="H8" s="12">
+      <c r="H8" s="14">
         <v>94.6</v>
       </c>
     </row>
@@ -1057,25 +1227,25 @@
       <c r="A9" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B9" s="4">
+      <c r="B9" s="5">
         <v>2002</v>
       </c>
-      <c r="C9" s="12">
+      <c r="C9" s="14">
         <v>622122</v>
       </c>
-      <c r="D9" s="12">
+      <c r="D9" s="14">
         <v>52.9</v>
       </c>
-      <c r="E9" s="11">
+      <c r="E9" s="13">
         <v>41.9</v>
       </c>
-      <c r="F9" s="12">
+      <c r="F9" s="14">
         <v>88.8</v>
       </c>
-      <c r="G9" s="12">
+      <c r="G9" s="14">
         <v>86.6</v>
       </c>
-      <c r="H9" s="12">
+      <c r="H9" s="14">
         <v>94.8</v>
       </c>
     </row>
@@ -1083,25 +1253,25 @@
       <c r="A10" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B10" s="4">
+      <c r="B10" s="5">
         <v>2003</v>
       </c>
-      <c r="C10" s="12">
+      <c r="C10" s="14">
         <v>643560</v>
       </c>
-      <c r="D10" s="12">
+      <c r="D10" s="14">
         <v>53.7</v>
       </c>
-      <c r="E10" s="11">
+      <c r="E10" s="13">
         <v>42.6</v>
       </c>
-      <c r="F10" s="12">
+      <c r="F10" s="14">
         <v>88.8</v>
       </c>
-      <c r="G10" s="12">
+      <c r="G10" s="14">
         <v>86.7</v>
       </c>
-      <c r="H10" s="12">
+      <c r="H10" s="14">
         <v>95.9</v>
       </c>
       <c r="I10" t="s">
@@ -1112,25 +1282,25 @@
       <c r="A11" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B11" s="5">
+      <c r="B11" s="6">
         <v>2004</v>
       </c>
-      <c r="C11" s="12">
+      <c r="C11" s="14">
         <v>636771</v>
       </c>
-      <c r="D11" s="12">
+      <c r="D11" s="14">
         <v>56.3</v>
       </c>
-      <c r="E11" s="11">
+      <c r="E11" s="13">
         <v>44.3</v>
       </c>
-      <c r="F11" s="12">
+      <c r="F11" s="14">
         <v>89</v>
       </c>
-      <c r="G11" s="12">
+      <c r="G11" s="14">
         <v>86.9</v>
       </c>
-      <c r="H11" s="12">
+      <c r="H11" s="14">
         <v>96.4</v>
       </c>
     </row>
@@ -1138,25 +1308,25 @@
       <c r="A12" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B12" s="5">
+      <c r="B12" s="6">
         <v>2005</v>
       </c>
-      <c r="C12" s="13">
+      <c r="C12" s="15">
         <v>648942</v>
       </c>
-      <c r="D12" s="13">
+      <c r="D12" s="15">
         <v>58.5</v>
       </c>
-      <c r="E12" s="17">
+      <c r="E12" s="19">
         <v>45.3</v>
       </c>
-      <c r="F12" s="13">
+      <c r="F12" s="15">
         <v>89.4</v>
       </c>
-      <c r="G12" s="13">
+      <c r="G12" s="15">
         <v>86.8</v>
       </c>
-      <c r="H12" s="13">
+      <c r="H12" s="15">
         <v>96.7</v>
       </c>
     </row>
@@ -1164,25 +1334,25 @@
       <c r="A13" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B13" s="5">
+      <c r="B13" s="6">
         <v>2006</v>
       </c>
-      <c r="C13" s="13">
+      <c r="C13" s="15">
         <v>656396</v>
       </c>
-      <c r="D13" s="13">
+      <c r="D13" s="15">
         <v>60.9</v>
       </c>
-      <c r="E13" s="17">
+      <c r="E13" s="19">
         <v>46</v>
       </c>
-      <c r="F13" s="13">
+      <c r="F13" s="15">
         <v>90</v>
       </c>
-      <c r="G13" s="13">
+      <c r="G13" s="15">
         <v>86.4</v>
       </c>
-      <c r="H13" s="13">
+      <c r="H13" s="15">
         <v>97.3</v>
       </c>
     </row>
@@ -1190,207 +1360,207 @@
       <c r="A14" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B14" s="5">
+      <c r="B14" s="6">
         <v>2007</v>
       </c>
-      <c r="C14" s="12">
+      <c r="C14" s="14">
         <v>653808</v>
       </c>
-      <c r="D14" s="12">
+      <c r="D14" s="14">
         <v>64.8</v>
       </c>
-      <c r="E14" s="12">
+      <c r="E14" s="14">
         <v>47.3</v>
       </c>
-      <c r="F14" s="12">
+      <c r="F14" s="14">
         <v>90.8</v>
       </c>
-      <c r="G14" s="12">
+      <c r="G14" s="14">
         <v>86.7</v>
       </c>
-      <c r="H14" s="12">
+      <c r="H14" s="14">
         <v>98</v>
       </c>
     </row>
     <row r="15" spans="1:9">
-      <c r="A15" s="6" t="s">
+      <c r="A15" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="B15" s="5">
+      <c r="B15" s="6">
         <v>2004</v>
       </c>
-      <c r="C15" s="13">
+      <c r="C15" s="15">
         <v>636119</v>
       </c>
-      <c r="D15" s="13">
+      <c r="D15" s="15">
         <v>56.8</v>
       </c>
-      <c r="E15" s="13">
+      <c r="E15" s="15">
         <v>44.7</v>
       </c>
-      <c r="F15" s="13">
+      <c r="F15" s="15">
         <v>89.9</v>
       </c>
-      <c r="G15" s="13">
+      <c r="G15" s="15">
         <v>87.6</v>
       </c>
-      <c r="H15" s="13">
+      <c r="H15" s="15">
         <v>97</v>
       </c>
     </row>
     <row r="16" spans="1:9">
-      <c r="A16" s="6" t="s">
+      <c r="A16" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="B16" s="5">
+      <c r="B16" s="6">
         <v>2005</v>
       </c>
-      <c r="C16" s="13">
+      <c r="C16" s="15">
         <v>648833</v>
       </c>
-      <c r="D16" s="13">
+      <c r="D16" s="15">
         <v>59</v>
       </c>
-      <c r="E16" s="13">
+      <c r="E16" s="15">
         <v>45.6</v>
       </c>
-      <c r="F16" s="13">
+      <c r="F16" s="15">
         <v>90.1</v>
       </c>
-      <c r="G16" s="13">
+      <c r="G16" s="15">
         <v>87.4</v>
       </c>
-      <c r="H16" s="13">
+      <c r="H16" s="15">
         <v>97.3</v>
       </c>
     </row>
     <row r="17" spans="1:9">
-      <c r="A17" s="6" t="s">
+      <c r="A17" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="B17" s="5">
+      <c r="B17" s="6">
         <v>2006</v>
       </c>
-      <c r="C17" s="13">
+      <c r="C17" s="15">
         <v>655146</v>
       </c>
-      <c r="D17" s="13">
+      <c r="D17" s="15">
         <v>61.4</v>
       </c>
-      <c r="E17" s="13">
+      <c r="E17" s="15">
         <v>46.3</v>
       </c>
-      <c r="F17" s="13">
+      <c r="F17" s="15">
         <v>90.9</v>
       </c>
-      <c r="G17" s="13">
+      <c r="G17" s="15">
         <v>87.1</v>
       </c>
-      <c r="H17" s="13">
+      <c r="H17" s="15">
         <v>98</v>
       </c>
     </row>
     <row r="18" spans="1:9">
-      <c r="A18" s="6" t="s">
+      <c r="A18" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="B18" s="5">
+      <c r="B18" s="6">
         <v>2007</v>
       </c>
-      <c r="C18" s="13">
+      <c r="C18" s="15">
         <v>653083</v>
       </c>
-      <c r="D18" s="13">
+      <c r="D18" s="15">
         <v>65.3</v>
       </c>
-      <c r="E18" s="13">
+      <c r="E18" s="15">
         <v>47.6</v>
       </c>
-      <c r="F18" s="13">
+      <c r="F18" s="15">
         <v>91.6</v>
       </c>
-      <c r="G18" s="13">
+      <c r="G18" s="15">
         <v>87.4</v>
       </c>
-      <c r="H18" s="13">
+      <c r="H18" s="15">
         <v>98.6</v>
       </c>
     </row>
     <row r="19" spans="1:9">
-      <c r="A19" s="6" t="s">
+      <c r="A19" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="B19" s="5">
+      <c r="B19" s="6">
         <v>2008</v>
       </c>
-      <c r="C19" s="13">
+      <c r="C19" s="15">
         <v>634496</v>
       </c>
-      <c r="D19" s="13">
+      <c r="D19" s="15">
         <v>70</v>
       </c>
-      <c r="E19" s="13">
+      <c r="E19" s="15">
         <v>49.8</v>
       </c>
-      <c r="F19" s="13">
+      <c r="F19" s="15">
         <v>92.3</v>
       </c>
-      <c r="G19" s="13">
+      <c r="G19" s="15">
         <v>88.3</v>
       </c>
-      <c r="H19" s="13">
+      <c r="H19" s="15">
         <v>98.9</v>
       </c>
     </row>
     <row r="20" spans="1:9">
-      <c r="A20" s="6" t="s">
+      <c r="A20" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="B20" s="7">
+      <c r="B20" s="9">
         <v>2009</v>
       </c>
-      <c r="C20" s="14">
+      <c r="C20" s="16">
         <v>639263</v>
       </c>
-      <c r="D20" s="14">
+      <c r="D20" s="16">
         <v>75.3</v>
       </c>
-      <c r="E20" s="14">
+      <c r="E20" s="16">
         <v>53.4</v>
       </c>
-      <c r="F20" s="14">
+      <c r="F20" s="16">
         <v>92.8</v>
       </c>
-      <c r="G20" s="14">
+      <c r="G20" s="16">
         <v>88.7</v>
       </c>
-      <c r="H20" s="14">
+      <c r="H20" s="16">
         <v>99</v>
       </c>
     </row>
     <row r="21" spans="1:9">
-      <c r="A21" s="6" t="s">
+      <c r="A21" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="B21" s="5">
+      <c r="B21" s="6">
         <v>2009</v>
       </c>
-      <c r="C21" s="13">
+      <c r="C21" s="15">
         <v>639263</v>
       </c>
-      <c r="D21" s="13">
+      <c r="D21" s="15">
         <v>75.400000000000006</v>
       </c>
-      <c r="E21" s="13">
+      <c r="E21" s="15">
         <v>53.5</v>
       </c>
-      <c r="F21" s="13">
+      <c r="F21" s="15">
         <v>92.9</v>
       </c>
-      <c r="G21" s="13">
+      <c r="G21" s="15">
         <v>88.8</v>
       </c>
-      <c r="H21" s="13">
+      <c r="H21" s="15">
         <v>99.1</v>
       </c>
       <c r="I21" t="s">
@@ -1398,262 +1568,262 @@
       </c>
     </row>
     <row r="22" spans="1:9">
-      <c r="A22" s="6" t="s">
+      <c r="A22" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="B22" s="5">
+      <c r="B22" s="6">
         <v>2010</v>
       </c>
-      <c r="C22" s="13">
+      <c r="C22" s="15">
         <v>627093</v>
       </c>
-      <c r="D22" s="13">
+      <c r="D22" s="15">
         <v>79.599999999999994</v>
       </c>
-      <c r="E22" s="13">
+      <c r="E22" s="15">
         <v>59</v>
       </c>
-      <c r="F22" s="13">
+      <c r="F22" s="15">
         <v>93.6</v>
       </c>
-      <c r="G22" s="13">
+      <c r="G22" s="15">
         <v>92.2</v>
       </c>
-      <c r="H22" s="13">
+      <c r="H22" s="15">
         <v>99.3</v>
       </c>
     </row>
     <row r="23" spans="1:9">
-      <c r="A23" s="6" t="s">
+      <c r="A23" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="B23" s="5">
+      <c r="B23" s="6">
         <v>2011</v>
       </c>
-      <c r="C23" s="13">
+      <c r="C23" s="15">
         <v>620617</v>
       </c>
-      <c r="D23" s="13">
+      <c r="D23" s="15">
         <v>81.900000000000006</v>
       </c>
-      <c r="E23" s="13">
+      <c r="E23" s="15">
         <v>59.4</v>
       </c>
-      <c r="F23" s="13">
+      <c r="F23" s="15">
         <v>94.1</v>
       </c>
-      <c r="G23" s="13">
+      <c r="G23" s="15">
         <v>92.5</v>
       </c>
-      <c r="H23" s="13">
+      <c r="H23" s="15">
         <v>99.6</v>
       </c>
     </row>
     <row r="24" spans="1:9">
-      <c r="A24" s="6" t="s">
+      <c r="A24" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="B24" s="5">
+      <c r="B24" s="6">
         <v>2012</v>
       </c>
-      <c r="C24" s="13">
+      <c r="C24" s="15">
         <v>632676</v>
       </c>
-      <c r="D24" s="13">
+      <c r="D24" s="15">
         <v>81.8</v>
       </c>
-      <c r="E24" s="13">
+      <c r="E24" s="15">
         <v>59.2</v>
       </c>
-      <c r="F24" s="13">
+      <c r="F24" s="15">
         <v>94.3</v>
       </c>
-      <c r="G24" s="13">
+      <c r="G24" s="15">
         <v>90.5</v>
       </c>
-      <c r="H24" s="13">
+      <c r="H24" s="15">
         <v>99.6</v>
       </c>
     </row>
     <row r="25" spans="1:9">
-      <c r="A25" s="8" t="s">
+      <c r="A25" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="B25" s="5">
+      <c r="B25" s="6">
         <v>2004</v>
       </c>
-      <c r="C25" s="13">
+      <c r="C25" s="15">
         <v>584170</v>
       </c>
-      <c r="D25" s="13">
+      <c r="D25" s="15">
         <v>54.9</v>
       </c>
-      <c r="E25" s="13">
+      <c r="E25" s="15">
         <v>42.5</v>
       </c>
-      <c r="F25" s="13">
+      <c r="F25" s="15">
         <v>90.3</v>
       </c>
-      <c r="G25" s="13">
+      <c r="G25" s="15">
         <v>88.5</v>
       </c>
-      <c r="H25" s="13">
+      <c r="H25" s="15">
         <v>97.3</v>
       </c>
     </row>
     <row r="26" spans="1:9">
-      <c r="A26" s="8" t="s">
+      <c r="A26" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="B26" s="5">
+      <c r="B26" s="6">
         <v>2005</v>
       </c>
-      <c r="C26" s="13">
+      <c r="C26" s="15">
         <v>594134</v>
       </c>
-      <c r="D26" s="13">
+      <c r="D26" s="15">
         <v>57.3</v>
       </c>
-      <c r="E26" s="13">
+      <c r="E26" s="15">
         <v>44</v>
       </c>
-      <c r="F26" s="13">
+      <c r="F26" s="15">
         <v>90.8</v>
       </c>
-      <c r="G26" s="13">
+      <c r="G26" s="15">
         <v>88.8</v>
       </c>
-      <c r="H26" s="13">
+      <c r="H26" s="15">
         <v>97.8</v>
       </c>
     </row>
     <row r="27" spans="1:9">
-      <c r="A27" s="8" t="s">
+      <c r="A27" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="B27" s="5">
+      <c r="B27" s="6">
         <v>2006</v>
       </c>
-      <c r="C27" s="13">
+      <c r="C27" s="15">
         <v>600664</v>
       </c>
-      <c r="D27" s="13">
+      <c r="D27" s="15">
         <v>59.9</v>
       </c>
-      <c r="E27" s="13">
+      <c r="E27" s="15">
         <v>45.8</v>
       </c>
-      <c r="F27" s="13">
+      <c r="F27" s="15">
         <v>91.5</v>
       </c>
-      <c r="G27" s="13">
+      <c r="G27" s="15">
         <v>89.6</v>
       </c>
-      <c r="H27" s="13">
+      <c r="H27" s="15">
         <v>98.4</v>
       </c>
     </row>
     <row r="28" spans="1:9">
-      <c r="A28" s="8" t="s">
+      <c r="A28" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="B28" s="5">
+      <c r="B28" s="6">
         <v>2007</v>
       </c>
-      <c r="C28" s="13">
+      <c r="C28" s="15">
         <v>598102</v>
       </c>
-      <c r="D28" s="13">
+      <c r="D28" s="15">
         <v>64.400000000000006</v>
       </c>
-      <c r="E28" s="13">
+      <c r="E28" s="15">
         <v>48.2</v>
       </c>
-      <c r="F28" s="13">
+      <c r="F28" s="15">
         <v>92.4</v>
       </c>
-      <c r="G28" s="13">
+      <c r="G28" s="15">
         <v>90.9</v>
       </c>
-      <c r="H28" s="13">
+      <c r="H28" s="15">
         <v>98.3</v>
       </c>
     </row>
     <row r="29" spans="1:9">
-      <c r="A29" s="8" t="s">
+      <c r="A29" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="B29" s="5">
+      <c r="B29" s="6">
         <v>2008</v>
       </c>
-      <c r="C29" s="13">
+      <c r="C29" s="15">
         <v>578841</v>
       </c>
-      <c r="D29" s="13">
+      <c r="D29" s="15">
         <v>69.8</v>
       </c>
-      <c r="E29" s="13">
+      <c r="E29" s="15">
         <v>50.7</v>
       </c>
-      <c r="F29" s="13">
+      <c r="F29" s="15">
         <v>93.5</v>
       </c>
-      <c r="G29" s="13">
+      <c r="G29" s="15">
         <v>92</v>
       </c>
-      <c r="H29" s="13">
+      <c r="H29" s="15">
         <v>98.7</v>
       </c>
     </row>
     <row r="30" spans="1:9">
-      <c r="A30" s="8" t="s">
+      <c r="A30" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="B30" s="7">
+      <c r="B30" s="9">
         <v>2009</v>
       </c>
-      <c r="C30" s="14">
+      <c r="C30" s="16">
         <v>578060</v>
       </c>
-      <c r="D30" s="14">
+      <c r="D30" s="16">
         <v>76.099999999999994</v>
       </c>
-      <c r="E30" s="14">
+      <c r="E30" s="16">
         <v>55.1</v>
       </c>
-      <c r="F30" s="14">
+      <c r="F30" s="16">
         <v>94.7</v>
       </c>
-      <c r="G30" s="14">
+      <c r="G30" s="16">
         <v>93.3</v>
       </c>
-      <c r="H30" s="14">
+      <c r="H30" s="16">
         <v>99</v>
       </c>
     </row>
     <row r="31" spans="1:9">
-      <c r="A31" s="8" t="s">
+      <c r="A31" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="B31" s="5">
+      <c r="B31" s="6">
         <v>2009</v>
       </c>
-      <c r="C31" s="13">
+      <c r="C31" s="15">
         <v>578060</v>
       </c>
-      <c r="D31" s="13">
+      <c r="D31" s="15">
         <v>76.099999999999994</v>
       </c>
-      <c r="E31" s="13">
+      <c r="E31" s="15">
         <v>55.1</v>
       </c>
-      <c r="F31" s="13">
+      <c r="F31" s="15">
         <v>94.7</v>
       </c>
-      <c r="G31" s="13">
+      <c r="G31" s="15">
         <v>93.3</v>
       </c>
-      <c r="H31" s="13">
+      <c r="H31" s="15">
         <v>99</v>
       </c>
       <c r="I31" t="s">
@@ -1661,80 +1831,80 @@
       </c>
     </row>
     <row r="32" spans="1:9">
-      <c r="A32" s="8" t="s">
+      <c r="A32" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="B32" s="5">
+      <c r="B32" s="6">
         <v>2010</v>
       </c>
-      <c r="C32" s="13">
+      <c r="C32" s="15">
         <v>566927</v>
       </c>
-      <c r="D32" s="13">
+      <c r="D32" s="15">
         <v>80.5</v>
       </c>
-      <c r="E32" s="13">
+      <c r="E32" s="15">
         <v>58.2</v>
       </c>
-      <c r="F32" s="13">
+      <c r="F32" s="15">
         <v>95.2</v>
       </c>
-      <c r="G32" s="13">
+      <c r="G32" s="15">
         <v>93.9</v>
       </c>
-      <c r="H32" s="13">
+      <c r="H32" s="15">
         <v>99.2</v>
       </c>
     </row>
     <row r="33" spans="1:8">
-      <c r="A33" s="8" t="s">
+      <c r="A33" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="B33" s="5">
+      <c r="B33" s="6">
         <v>2011</v>
       </c>
-      <c r="C33" s="13">
+      <c r="C33" s="15">
         <v>561308</v>
       </c>
-      <c r="D33" s="13">
+      <c r="D33" s="15">
         <v>83</v>
       </c>
-      <c r="E33" s="13">
+      <c r="E33" s="15">
         <v>58.8</v>
       </c>
-      <c r="F33" s="13">
+      <c r="F33" s="15">
         <v>95.7</v>
       </c>
-      <c r="G33" s="13">
+      <c r="G33" s="15">
         <v>94.2</v>
       </c>
-      <c r="H33" s="13">
+      <c r="H33" s="15">
         <v>99.3</v>
       </c>
     </row>
     <row r="34" spans="1:8">
-      <c r="A34" s="8" t="s">
+      <c r="A34" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="B34" s="5">
+      <c r="B34" s="6">
         <v>2012</v>
       </c>
-      <c r="C34" s="13">
+      <c r="C34" s="15">
         <v>571334</v>
       </c>
-      <c r="D34" s="13">
+      <c r="D34" s="15">
         <v>82.9</v>
       </c>
-      <c r="E34" s="13">
+      <c r="E34" s="15">
         <v>60.6</v>
       </c>
-      <c r="F34" s="13">
+      <c r="F34" s="15">
         <v>95.8</v>
       </c>
-      <c r="G34" s="13">
+      <c r="G34" s="15">
         <v>94.2</v>
       </c>
-      <c r="H34" s="13">
+      <c r="H34" s="15">
         <v>99.3</v>
       </c>
     </row>
@@ -1753,254 +1923,660 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y4"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="16384" width="10.83203125" style="17"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:25" ht="30">
+      <c r="A1" s="31" t="s">
+        <v>48</v>
+      </c>
+      <c r="B1" s="32" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" s="32" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" s="33" t="s">
+        <v>19</v>
+      </c>
+      <c r="E1" s="33" t="s">
+        <v>20</v>
+      </c>
+      <c r="F1" s="33" t="s">
+        <v>21</v>
+      </c>
+      <c r="G1" s="33" t="s">
+        <v>22</v>
+      </c>
+      <c r="H1" s="33" t="s">
+        <v>23</v>
+      </c>
+      <c r="I1" s="33" t="s">
+        <v>24</v>
+      </c>
+      <c r="J1" s="34" t="s">
+        <v>25</v>
+      </c>
+      <c r="K1" s="34" t="s">
+        <v>26</v>
+      </c>
+      <c r="L1" s="35" t="s">
+        <v>27</v>
+      </c>
+      <c r="M1" s="35" t="s">
+        <v>28</v>
+      </c>
+      <c r="N1" s="35" t="s">
+        <v>29</v>
+      </c>
+      <c r="O1" s="35" t="s">
+        <v>30</v>
+      </c>
+      <c r="P1" s="35" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q1" s="35" t="s">
+        <v>32</v>
+      </c>
+      <c r="R1" s="36" t="s">
+        <v>33</v>
+      </c>
+      <c r="S1" s="36" t="s">
+        <v>34</v>
+      </c>
+      <c r="T1" s="36" t="s">
+        <v>35</v>
+      </c>
+      <c r="U1" s="36" t="s">
+        <v>36</v>
+      </c>
+      <c r="V1" s="36" t="s">
+        <v>37</v>
+      </c>
+      <c r="W1" s="36" t="s">
+        <v>38</v>
+      </c>
+      <c r="X1" s="36" t="s">
+        <v>39</v>
+      </c>
+      <c r="Y1" s="36" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="2" spans="1:25">
+      <c r="A2" s="37" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" s="15">
+        <v>328005</v>
+      </c>
+      <c r="C2" s="15">
+        <v>321415</v>
+      </c>
+      <c r="D2" s="15">
+        <v>318599</v>
+      </c>
+      <c r="E2" s="15">
+        <v>323971</v>
+      </c>
+      <c r="F2" s="15">
+        <v>294465</v>
+      </c>
+      <c r="G2" s="15">
+        <v>288885</v>
+      </c>
+      <c r="H2" s="15">
+        <v>286652</v>
+      </c>
+      <c r="I2" s="15">
+        <v>291008</v>
+      </c>
+      <c r="J2" s="20">
+        <v>19.600000000000001</v>
+      </c>
+      <c r="K2" s="20">
+        <v>21.4</v>
+      </c>
+      <c r="L2" s="20">
+        <v>22.7</v>
+      </c>
+      <c r="M2" s="15">
+        <v>30.6</v>
+      </c>
+      <c r="N2" s="13">
+        <v>19.8</v>
+      </c>
+      <c r="O2" s="20">
+        <v>19.399999999999999</v>
+      </c>
+      <c r="P2" s="20">
+        <v>20.7</v>
+      </c>
+      <c r="Q2" s="15">
+        <v>31.5</v>
+      </c>
+      <c r="R2" s="14">
+        <v>12.8</v>
+      </c>
+      <c r="S2" s="20">
+        <v>14.8</v>
+      </c>
+      <c r="T2" s="20">
+        <v>15.5</v>
+      </c>
+      <c r="U2" s="15">
+        <v>18.3</v>
+      </c>
+      <c r="V2" s="13">
+        <v>12.6</v>
+      </c>
+      <c r="W2" s="20">
+        <v>12.7</v>
+      </c>
+      <c r="X2" s="20">
+        <v>13.3</v>
+      </c>
+      <c r="Y2" s="15">
+        <v>18.3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:25">
+      <c r="A3" s="37" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" s="15">
+        <v>311258</v>
+      </c>
+      <c r="C3" s="15">
+        <v>305678</v>
+      </c>
+      <c r="D3" s="15">
+        <v>302018</v>
+      </c>
+      <c r="E3" s="15">
+        <v>308705</v>
+      </c>
+      <c r="F3" s="15">
+        <v>283595</v>
+      </c>
+      <c r="G3" s="15">
+        <v>278042</v>
+      </c>
+      <c r="H3" s="15">
+        <v>274656</v>
+      </c>
+      <c r="I3" s="15">
+        <v>280326</v>
+      </c>
+      <c r="J3" s="20">
+        <v>24.5</v>
+      </c>
+      <c r="K3" s="20">
+        <v>26.3</v>
+      </c>
+      <c r="L3" s="20">
+        <v>27.8</v>
+      </c>
+      <c r="M3" s="15">
+        <v>39.299999999999997</v>
+      </c>
+      <c r="N3" s="13">
+        <v>24</v>
+      </c>
+      <c r="O3" s="20">
+        <v>23.9</v>
+      </c>
+      <c r="P3" s="20">
+        <v>25.6</v>
+      </c>
+      <c r="Q3" s="15">
+        <v>39.6</v>
+      </c>
+      <c r="R3" s="14">
+        <v>18.5</v>
+      </c>
+      <c r="S3" s="20">
+        <v>20.6</v>
+      </c>
+      <c r="T3" s="20">
+        <v>21.4</v>
+      </c>
+      <c r="U3" s="15">
+        <v>27.8</v>
+      </c>
+      <c r="V3" s="13">
+        <v>17.7</v>
+      </c>
+      <c r="W3" s="20">
+        <v>18.2</v>
+      </c>
+      <c r="X3" s="20">
+        <v>19.100000000000001</v>
+      </c>
+      <c r="Y3" s="15">
+        <v>27.5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:25">
+      <c r="A4" s="33"/>
+      <c r="B4" s="13"/>
+      <c r="C4" s="33"/>
+      <c r="D4" s="33"/>
+      <c r="E4" s="38"/>
+      <c r="F4" s="33"/>
+      <c r="G4" s="32"/>
+      <c r="H4" s="32"/>
+      <c r="I4" s="15"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:Q8"/>
+  <sheetViews>
+    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="16384" width="10.83203125" style="15"/>
+    <col min="1" max="1" width="36.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" ht="30">
-      <c r="A1" s="19"/>
-      <c r="B1" s="20" t="s">
-        <v>17</v>
-      </c>
-      <c r="C1" s="20" t="s">
-        <v>18</v>
-      </c>
-      <c r="D1" s="21" t="s">
-        <v>19</v>
-      </c>
-      <c r="E1" s="21" t="s">
-        <v>20</v>
-      </c>
-      <c r="F1" s="21" t="s">
-        <v>21</v>
-      </c>
-      <c r="G1" s="21" t="s">
-        <v>22</v>
-      </c>
-      <c r="H1" s="21" t="s">
-        <v>23</v>
-      </c>
-      <c r="I1" s="21" t="s">
-        <v>24</v>
+    <row r="1" spans="1:17" ht="30">
+      <c r="A1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B1" s="22" t="s">
+        <v>25</v>
+      </c>
+      <c r="C1" s="22" t="s">
+        <v>26</v>
+      </c>
+      <c r="D1" s="22" t="s">
+        <v>27</v>
+      </c>
+      <c r="E1" s="22" t="s">
+        <v>28</v>
+      </c>
+      <c r="F1" s="22" t="s">
+        <v>29</v>
+      </c>
+      <c r="G1" s="22" t="s">
+        <v>30</v>
+      </c>
+      <c r="H1" s="22" t="s">
+        <v>31</v>
+      </c>
+      <c r="I1" s="22" t="s">
+        <v>32</v>
       </c>
       <c r="J1" s="22" t="s">
-        <v>25</v>
+        <v>33</v>
       </c>
       <c r="K1" s="22" t="s">
-        <v>26</v>
-      </c>
-      <c r="L1" s="23" t="s">
-        <v>27</v>
-      </c>
-      <c r="M1" s="23" t="s">
-        <v>28</v>
-      </c>
-      <c r="N1" s="23" t="s">
-        <v>29</v>
-      </c>
-      <c r="O1" s="23" t="s">
-        <v>30</v>
-      </c>
-      <c r="P1" s="23" t="s">
-        <v>31</v>
-      </c>
-      <c r="Q1" s="23" t="s">
-        <v>32</v>
-      </c>
-      <c r="R1" s="24" t="s">
-        <v>33</v>
-      </c>
-      <c r="S1" s="24" t="s">
         <v>34</v>
       </c>
-      <c r="T1" s="24" t="s">
+      <c r="L1" s="22" t="s">
         <v>35</v>
       </c>
-      <c r="U1" s="24" t="s">
+      <c r="M1" s="22" t="s">
         <v>36</v>
       </c>
-      <c r="V1" s="24" t="s">
+      <c r="N1" s="22" t="s">
         <v>37</v>
       </c>
-      <c r="W1" s="24" t="s">
+      <c r="O1" s="22" t="s">
         <v>38</v>
       </c>
-      <c r="X1" s="24" t="s">
+      <c r="P1" s="22" t="s">
         <v>39</v>
       </c>
-      <c r="Y1" s="24" t="s">
+      <c r="Q1" s="22" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="2" spans="1:25">
-      <c r="A2" s="25" t="s">
-        <v>15</v>
-      </c>
-      <c r="B2" s="13">
-        <v>328005</v>
-      </c>
-      <c r="C2" s="13">
-        <v>321415</v>
-      </c>
-      <c r="D2" s="13">
-        <v>318599</v>
-      </c>
-      <c r="E2" s="13">
-        <v>323971</v>
-      </c>
-      <c r="F2" s="13">
-        <v>294465</v>
-      </c>
-      <c r="G2" s="13">
-        <v>288885</v>
-      </c>
-      <c r="H2" s="13">
-        <v>286652</v>
-      </c>
-      <c r="I2" s="13">
-        <v>291008</v>
-      </c>
-      <c r="J2" s="18">
-        <v>19.600000000000001</v>
-      </c>
-      <c r="K2" s="18">
-        <v>21.4</v>
-      </c>
-      <c r="L2" s="18">
-        <v>22.7</v>
-      </c>
-      <c r="M2" s="13">
-        <v>30.6</v>
-      </c>
-      <c r="N2" s="11">
-        <v>19.8</v>
-      </c>
-      <c r="O2" s="18">
-        <v>19.399999999999999</v>
-      </c>
-      <c r="P2" s="18">
-        <v>20.7</v>
-      </c>
-      <c r="Q2" s="13">
-        <v>31.5</v>
-      </c>
-      <c r="R2" s="12">
-        <v>12.8</v>
-      </c>
-      <c r="S2" s="18">
-        <v>14.8</v>
-      </c>
-      <c r="T2" s="18">
-        <v>15.5</v>
-      </c>
-      <c r="U2" s="13">
-        <v>18.3</v>
-      </c>
-      <c r="V2" s="11">
-        <v>12.6</v>
-      </c>
-      <c r="W2" s="18">
-        <v>12.7</v>
-      </c>
-      <c r="X2" s="18">
-        <v>13.3</v>
-      </c>
-      <c r="Y2" s="13">
-        <v>18.3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:25">
-      <c r="A3" s="25" t="s">
-        <v>16</v>
-      </c>
-      <c r="B3" s="13">
-        <v>311258</v>
-      </c>
-      <c r="C3" s="13">
-        <v>305678</v>
-      </c>
-      <c r="D3" s="13">
-        <v>302018</v>
-      </c>
-      <c r="E3" s="13">
-        <v>308705</v>
-      </c>
-      <c r="F3" s="13">
-        <v>283595</v>
-      </c>
-      <c r="G3" s="13">
-        <v>278042</v>
-      </c>
-      <c r="H3" s="13">
-        <v>274656</v>
-      </c>
-      <c r="I3" s="13">
-        <v>280326</v>
-      </c>
-      <c r="J3" s="18">
-        <v>24.5</v>
-      </c>
-      <c r="K3" s="18">
-        <v>26.3</v>
-      </c>
-      <c r="L3" s="18">
-        <v>27.8</v>
-      </c>
-      <c r="M3" s="13">
-        <v>39.299999999999997</v>
-      </c>
-      <c r="N3" s="11">
-        <v>24</v>
-      </c>
-      <c r="O3" s="18">
-        <v>23.9</v>
-      </c>
-      <c r="P3" s="18">
-        <v>25.6</v>
-      </c>
-      <c r="Q3" s="13">
+    <row r="2" spans="1:17">
+      <c r="A2" s="23" t="s">
+        <v>41</v>
+      </c>
+      <c r="B2" s="4">
+        <v>94.4</v>
+      </c>
+      <c r="C2" s="4">
+        <v>95</v>
+      </c>
+      <c r="D2" s="21">
+        <v>94.9</v>
+      </c>
+      <c r="E2" s="7">
+        <v>93.1</v>
+      </c>
+      <c r="F2" s="4">
+        <v>95.9</v>
+      </c>
+      <c r="G2" s="4">
+        <v>96.3</v>
+      </c>
+      <c r="H2" s="21">
+        <v>96.4</v>
+      </c>
+      <c r="I2" s="7">
+        <v>96.6</v>
+      </c>
+      <c r="J2" s="4">
+        <v>66.2</v>
+      </c>
+      <c r="K2" s="4">
+        <v>69.099999999999994</v>
+      </c>
+      <c r="L2" s="21">
+        <v>66.900000000000006</v>
+      </c>
+      <c r="M2" s="7">
+        <v>66.400000000000006</v>
+      </c>
+      <c r="N2" s="4">
+        <v>65.8</v>
+      </c>
+      <c r="O2" s="4">
+        <v>68.7</v>
+      </c>
+      <c r="P2" s="21">
+        <v>66.7</v>
+      </c>
+      <c r="Q2" s="7">
+        <v>68.3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17">
+      <c r="A3" s="23" t="s">
+        <v>42</v>
+      </c>
+      <c r="B3" s="4">
+        <v>93.1</v>
+      </c>
+      <c r="C3" s="4">
+        <v>96.2</v>
+      </c>
+      <c r="D3" s="21">
+        <v>96.7</v>
+      </c>
+      <c r="E3" s="7">
+        <v>96.8</v>
+      </c>
+      <c r="F3" s="4">
+        <v>97</v>
+      </c>
+      <c r="G3" s="4">
+        <v>97.3</v>
+      </c>
+      <c r="H3" s="21">
+        <v>97.5</v>
+      </c>
+      <c r="I3" s="7">
+        <v>97.6</v>
+      </c>
+      <c r="J3" s="4">
+        <v>60.6</v>
+      </c>
+      <c r="K3" s="4">
+        <v>65.900000000000006</v>
+      </c>
+      <c r="L3" s="21">
+        <v>69.8</v>
+      </c>
+      <c r="M3" s="7">
+        <v>71.5</v>
+      </c>
+      <c r="N3" s="4">
+        <v>62.4</v>
+      </c>
+      <c r="O3" s="4">
+        <v>65.2</v>
+      </c>
+      <c r="P3" s="21">
+        <v>69.3</v>
+      </c>
+      <c r="Q3" s="7">
+        <v>71.3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17">
+      <c r="A4" s="23" t="s">
+        <v>44</v>
+      </c>
+      <c r="B4" s="4">
+        <v>44.900000000000006</v>
+      </c>
+      <c r="C4" s="4">
+        <v>40.4</v>
+      </c>
+      <c r="D4" s="4">
         <v>39.6</v>
       </c>
-      <c r="R3" s="12">
-        <v>18.5</v>
-      </c>
-      <c r="S3" s="18">
-        <v>20.6</v>
-      </c>
-      <c r="T3" s="18">
-        <v>21.4</v>
-      </c>
-      <c r="U3" s="13">
-        <v>27.8</v>
-      </c>
-      <c r="V3" s="11">
-        <v>17.7</v>
-      </c>
-      <c r="W3" s="18">
-        <v>18.2</v>
-      </c>
-      <c r="X3" s="18">
-        <v>19.100000000000001</v>
-      </c>
-      <c r="Y3" s="13">
+      <c r="E4" s="4">
+        <v>39.899999999999991</v>
+      </c>
+      <c r="F4" s="4">
+        <v>44</v>
+      </c>
+      <c r="G4" s="4">
+        <v>37.700000000000003</v>
+      </c>
+      <c r="H4" s="4">
+        <v>36.799999999999997</v>
+      </c>
+      <c r="I4" s="4">
+        <v>37.9</v>
+      </c>
+      <c r="J4" s="4">
+        <v>48.400000000000006</v>
+      </c>
+      <c r="K4" s="4">
+        <v>45.500000000000007</v>
+      </c>
+      <c r="L4" s="4">
+        <v>42.500000000000007</v>
+      </c>
+      <c r="M4" s="4">
+        <v>28.300000000000004</v>
+      </c>
+      <c r="N4" s="4">
+        <v>44.599999999999994</v>
+      </c>
+      <c r="O4" s="4">
+        <v>40.200000000000003</v>
+      </c>
+      <c r="P4" s="4">
+        <v>37</v>
+      </c>
+      <c r="Q4" s="4">
+        <v>21.1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17">
+      <c r="A5" s="24" t="s">
+        <v>45</v>
+      </c>
+      <c r="B5" s="25">
+        <v>17.3</v>
+      </c>
+      <c r="C5" s="25">
+        <v>21.5</v>
+      </c>
+      <c r="D5" s="26">
+        <v>24.6</v>
+      </c>
+      <c r="E5" s="27">
+        <v>25.7</v>
+      </c>
+      <c r="F5" s="25">
+        <v>19.2</v>
+      </c>
+      <c r="G5" s="25">
+        <v>23.8</v>
+      </c>
+      <c r="H5" s="26">
+        <v>27.2</v>
+      </c>
+      <c r="I5" s="27">
+        <v>28.4</v>
+      </c>
+      <c r="J5" s="25">
+        <v>25.3</v>
+      </c>
+      <c r="K5" s="25">
+        <v>31.4</v>
+      </c>
+      <c r="L5" s="26">
+        <v>34.4</v>
+      </c>
+      <c r="M5" s="27">
+        <v>45.9</v>
+      </c>
+      <c r="N5" s="25">
         <v>27.5</v>
       </c>
-    </row>
-    <row r="4" spans="1:25">
-      <c r="A4" s="21"/>
-      <c r="B4" s="11"/>
-      <c r="C4" s="21"/>
-      <c r="D4" s="21"/>
-      <c r="E4" s="26"/>
-      <c r="F4" s="21"/>
-      <c r="G4" s="20"/>
-      <c r="H4" s="20"/>
-      <c r="I4" s="13"/>
+      <c r="O5" s="25">
+        <v>35</v>
+      </c>
+      <c r="P5" s="26">
+        <v>38.200000000000003</v>
+      </c>
+      <c r="Q5" s="27">
+        <v>51.4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17">
+      <c r="A6" s="28" t="s">
+        <v>46</v>
+      </c>
+      <c r="B6" s="4">
+        <v>48.9</v>
+      </c>
+      <c r="C6" s="4">
+        <v>48.9</v>
+      </c>
+      <c r="D6" s="21">
+        <v>50.4</v>
+      </c>
+      <c r="E6" s="7">
+        <v>60.4</v>
+      </c>
+      <c r="F6" s="4">
+        <v>47.7</v>
+      </c>
+      <c r="G6" s="4">
+        <v>47.9</v>
+      </c>
+      <c r="H6" s="21">
+        <v>49.3</v>
+      </c>
+      <c r="I6" s="7">
+        <v>60.2</v>
+      </c>
+      <c r="J6" s="4">
+        <v>69.8</v>
+      </c>
+      <c r="K6" s="4">
+        <v>70.5</v>
+      </c>
+      <c r="L6" s="21">
+        <v>70.7</v>
+      </c>
+      <c r="M6" s="7">
+        <v>69.5</v>
+      </c>
+      <c r="N6" s="4">
+        <v>66.7</v>
+      </c>
+      <c r="O6" s="4">
+        <v>67.7</v>
+      </c>
+      <c r="P6" s="21">
+        <v>68</v>
+      </c>
+      <c r="Q6" s="7">
+        <v>67.099999999999994</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17">
+      <c r="A7" s="23" t="s">
+        <v>47</v>
+      </c>
+      <c r="B7" s="4">
+        <v>42.6</v>
+      </c>
+      <c r="C7" s="4">
+        <v>40.9</v>
+      </c>
+      <c r="D7" s="21">
+        <v>41.1</v>
+      </c>
+      <c r="E7" s="7">
+        <v>48.7</v>
+      </c>
+      <c r="F7" s="4">
+        <v>40</v>
+      </c>
+      <c r="G7" s="4">
+        <v>38.5</v>
+      </c>
+      <c r="H7" s="21">
+        <v>38.9</v>
+      </c>
+      <c r="I7" s="7">
+        <v>47.6</v>
+      </c>
+      <c r="J7" s="4">
+        <v>72.599999999999994</v>
+      </c>
+      <c r="K7" s="4">
+        <v>73.599999999999994</v>
+      </c>
+      <c r="L7" s="21">
+        <v>73.599999999999994</v>
+      </c>
+      <c r="M7" s="7">
+        <v>72</v>
+      </c>
+      <c r="N7" s="4">
+        <v>69.3</v>
+      </c>
+      <c r="O7" s="4">
+        <v>70.599999999999994</v>
+      </c>
+      <c r="P7" s="21">
+        <v>70.7</v>
+      </c>
+      <c r="Q7" s="7">
+        <v>69.400000000000006</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17">
+      <c r="A8" s="30"/>
+      <c r="B8" s="4"/>
+      <c r="C8" s="29"/>
+      <c r="D8" s="29"/>
+      <c r="E8" s="29"/>
+      <c r="F8" s="29"/>
+      <c r="G8" s="29"/>
+      <c r="H8" s="29"/>
+      <c r="I8" s="29"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Forgot the "notes"column in the metadata
</commit_message>
<xml_diff>
--- a/data/processed/01_stage_1/SFR01_2014_NT.xlsx
+++ b/data/processed/01_stage_1/SFR01_2014_NT.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24030"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="2820" yWindow="0" windowWidth="25600" windowHeight="17480" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="2820" yWindow="0" windowWidth="25600" windowHeight="17480" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="table_1a.csv" sheetId="1" r:id="rId1"/>
@@ -32,9 +32,6 @@
     <t>Pupils at end Key Stage 4 in State-funded schools</t>
   </si>
   <si>
-    <t>Notes</t>
-  </si>
-  <si>
     <t>Percentages from 1996/97 include GCSEs and GNVQs.</t>
   </si>
   <si>
@@ -180,6 +177,9 @@
   </si>
   <si>
     <t>gender</t>
+  </si>
+  <si>
+    <t>notes</t>
   </si>
 </sst>
 </file>
@@ -997,8 +997,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I34"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="B35" sqref="B35"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1011,31 +1011,31 @@
   <sheetData>
     <row r="1" spans="1:9" ht="30">
       <c r="A1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="C1" s="12" t="s">
+      <c r="D1" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="D1" s="18" t="s">
+      <c r="E1" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="E1" s="18" t="s">
+      <c r="F1" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="F1" s="18" t="s">
+      <c r="G1" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="G1" s="18" t="s">
+      <c r="H1" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="H1" s="18" t="s">
-        <v>14</v>
-      </c>
       <c r="I1" s="11" t="s">
-        <v>3</v>
+        <v>48</v>
       </c>
     </row>
     <row r="2" spans="1:9">
@@ -1064,7 +1064,7 @@
         <v>92.2</v>
       </c>
       <c r="I2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:9">
@@ -1275,7 +1275,7 @@
         <v>95.9</v>
       </c>
       <c r="I10" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="11" spans="1:9">
@@ -1564,7 +1564,7 @@
         <v>99.1</v>
       </c>
       <c r="I21" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="22" spans="1:9">
@@ -1827,7 +1827,7 @@
         <v>99</v>
       </c>
       <c r="I31" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="32" spans="1:9">
@@ -1923,7 +1923,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y4"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0"/>
+    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
@@ -1932,84 +1932,84 @@
   <sheetData>
     <row r="1" spans="1:25" ht="30">
       <c r="A1" s="31" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B1" s="32" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" s="32" t="s">
         <v>17</v>
       </c>
-      <c r="C1" s="32" t="s">
+      <c r="D1" s="33" t="s">
         <v>18</v>
       </c>
-      <c r="D1" s="33" t="s">
+      <c r="E1" s="33" t="s">
         <v>19</v>
       </c>
-      <c r="E1" s="33" t="s">
+      <c r="F1" s="33" t="s">
         <v>20</v>
       </c>
-      <c r="F1" s="33" t="s">
+      <c r="G1" s="33" t="s">
         <v>21</v>
       </c>
-      <c r="G1" s="33" t="s">
+      <c r="H1" s="33" t="s">
         <v>22</v>
       </c>
-      <c r="H1" s="33" t="s">
+      <c r="I1" s="33" t="s">
         <v>23</v>
       </c>
-      <c r="I1" s="33" t="s">
+      <c r="J1" s="34" t="s">
         <v>24</v>
       </c>
-      <c r="J1" s="34" t="s">
+      <c r="K1" s="34" t="s">
         <v>25</v>
       </c>
-      <c r="K1" s="34" t="s">
+      <c r="L1" s="35" t="s">
         <v>26</v>
       </c>
-      <c r="L1" s="35" t="s">
+      <c r="M1" s="35" t="s">
         <v>27</v>
       </c>
-      <c r="M1" s="35" t="s">
+      <c r="N1" s="35" t="s">
         <v>28</v>
       </c>
-      <c r="N1" s="35" t="s">
+      <c r="O1" s="35" t="s">
         <v>29</v>
       </c>
-      <c r="O1" s="35" t="s">
+      <c r="P1" s="35" t="s">
         <v>30</v>
       </c>
-      <c r="P1" s="35" t="s">
+      <c r="Q1" s="35" t="s">
         <v>31</v>
       </c>
-      <c r="Q1" s="35" t="s">
+      <c r="R1" s="36" t="s">
         <v>32</v>
       </c>
-      <c r="R1" s="36" t="s">
+      <c r="S1" s="36" t="s">
         <v>33</v>
       </c>
-      <c r="S1" s="36" t="s">
+      <c r="T1" s="36" t="s">
         <v>34</v>
       </c>
-      <c r="T1" s="36" t="s">
+      <c r="U1" s="36" t="s">
         <v>35</v>
       </c>
-      <c r="U1" s="36" t="s">
+      <c r="V1" s="36" t="s">
         <v>36</v>
       </c>
-      <c r="V1" s="36" t="s">
+      <c r="W1" s="36" t="s">
         <v>37</v>
       </c>
-      <c r="W1" s="36" t="s">
+      <c r="X1" s="36" t="s">
         <v>38</v>
       </c>
-      <c r="X1" s="36" t="s">
+      <c r="Y1" s="36" t="s">
         <v>39</v>
-      </c>
-      <c r="Y1" s="36" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="2" spans="1:25">
       <c r="A2" s="37" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B2" s="15">
         <v>328005</v>
@@ -2086,7 +2086,7 @@
     </row>
     <row r="3" spans="1:25">
       <c r="A3" s="37" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B3" s="15">
         <v>311258</v>
@@ -2198,60 +2198,60 @@
   <sheetData>
     <row r="1" spans="1:17" ht="30">
       <c r="A1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B1" s="22" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1" s="22" t="s">
         <v>25</v>
       </c>
-      <c r="C1" s="22" t="s">
+      <c r="D1" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="D1" s="22" t="s">
+      <c r="E1" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="E1" s="22" t="s">
+      <c r="F1" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="F1" s="22" t="s">
+      <c r="G1" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="G1" s="22" t="s">
+      <c r="H1" s="22" t="s">
         <v>30</v>
       </c>
-      <c r="H1" s="22" t="s">
+      <c r="I1" s="22" t="s">
         <v>31</v>
       </c>
-      <c r="I1" s="22" t="s">
+      <c r="J1" s="22" t="s">
         <v>32</v>
       </c>
-      <c r="J1" s="22" t="s">
+      <c r="K1" s="22" t="s">
         <v>33</v>
       </c>
-      <c r="K1" s="22" t="s">
+      <c r="L1" s="22" t="s">
         <v>34</v>
       </c>
-      <c r="L1" s="22" t="s">
+      <c r="M1" s="22" t="s">
         <v>35</v>
       </c>
-      <c r="M1" s="22" t="s">
+      <c r="N1" s="22" t="s">
         <v>36</v>
       </c>
-      <c r="N1" s="22" t="s">
+      <c r="O1" s="22" t="s">
         <v>37</v>
       </c>
-      <c r="O1" s="22" t="s">
+      <c r="P1" s="22" t="s">
         <v>38</v>
       </c>
-      <c r="P1" s="22" t="s">
+      <c r="Q1" s="22" t="s">
         <v>39</v>
-      </c>
-      <c r="Q1" s="22" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="2" spans="1:17">
       <c r="A2" s="23" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B2" s="4">
         <v>94.4</v>
@@ -2304,7 +2304,7 @@
     </row>
     <row r="3" spans="1:17">
       <c r="A3" s="23" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B3" s="4">
         <v>93.1</v>
@@ -2357,7 +2357,7 @@
     </row>
     <row r="4" spans="1:17">
       <c r="A4" s="23" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B4" s="4">
         <v>44.900000000000006</v>
@@ -2410,7 +2410,7 @@
     </row>
     <row r="5" spans="1:17">
       <c r="A5" s="24" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B5" s="25">
         <v>17.3</v>
@@ -2463,7 +2463,7 @@
     </row>
     <row r="6" spans="1:17">
       <c r="A6" s="28" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B6" s="4">
         <v>48.9</v>
@@ -2516,7 +2516,7 @@
     </row>
     <row r="7" spans="1:17">
       <c r="A7" s="23" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B7" s="4">
         <v>42.6</v>

</xml_diff>